<commit_message>
House heating - Changed baud rate to 1500000 - Added happiness, outdoor temp - sima függvény hekkelés - SetDAC szépen belőve
</commit_message>
<xml_diff>
--- a/LabView/House heating/temp_out scaling.xlsx
+++ b/LabView/House heating/temp_out scaling.xlsx
@@ -21,6 +21,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>Volts</t>
+  </si>
+  <si>
+    <t>MADAQ</t>
+  </si>
+  <si>
+    <t>STICK</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -197,7 +214,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Munka1!$A$1:$A$2</c:f>
+              <c:f>Munka1!$B$2:$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -212,7 +229,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Munka1!$B$1:$B$2</c:f>
+              <c:f>Munka1!$C$2:$C$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -235,11 +252,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="998559296"/>
-        <c:axId val="998559840"/>
+        <c:axId val="-583674544"/>
+        <c:axId val="-583669104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="998559296"/>
+        <c:axId val="-583674544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -296,12 +313,12 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="998559840"/>
+        <c:crossAx val="-583669104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="998559840"/>
+        <c:axId val="-583669104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -358,7 +375,340 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="998559296"/>
+        <c:crossAx val="-583674544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="hu-HU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="hu-HU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="hu-HU"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Munka1!$B$5:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Munka1!$C$5:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-504596032"/>
+        <c:axId val="-504610176"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-504596032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-504610176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-504610176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-504596032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -447,7 +797,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -968,15 +1874,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -990,6 +1896,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagram 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1261,28 +2197,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2">
         <v>-10</v>
       </c>
-      <c r="B1">
+      <c r="C2">
         <v>-5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3">
         <v>40</v>
       </c>
-      <c r="B2">
+      <c r="C3">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>-10</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
House heating - Fixed: kit-en nem lehet negatív feszt mérni - Added: v0 vizsgafeladat for students
</commit_message>
<xml_diff>
--- a/LabView/House heating/temp_out scaling.xlsx
+++ b/LabView/House heating/temp_out scaling.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hallgato\Desktop\Bence\LabView\House heating\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11745"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -41,8 +36,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,7 +71,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -93,21 +88,10 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="hu-HU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -136,12 +120,10 @@
         </a:p>
       </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -178,7 +160,6 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout/>
@@ -219,10 +200,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-10</c:v>
+                  <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -234,7 +215,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
@@ -242,25 +223,16 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-583674544"/>
-        <c:axId val="-583669104"/>
+        <c:dLbls/>
+        <c:axId val="89748608"/>
+        <c:axId val="89750144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-583674544"/>
+        <c:axId val="89748608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -278,7 +250,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -313,16 +284,15 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-583669104"/>
+        <c:crossAx val="89750144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-583669104"/>
+        <c:axId val="89750144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -340,7 +310,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -375,7 +344,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-583674544"/>
+        <c:crossAx val="89748608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -389,7 +358,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -418,7 +386,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -426,21 +394,10 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="hu-HU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -469,12 +426,10 @@
         </a:p>
       </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -511,7 +466,6 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout/>
@@ -552,10 +506,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-10</c:v>
+                  <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -575,25 +529,16 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-504596032"/>
-        <c:axId val="-504610176"/>
+        <c:dLbls/>
+        <c:axId val="92744704"/>
+        <c:axId val="92746496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-504596032"/>
+        <c:axId val="92744704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -611,7 +556,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -646,16 +590,15 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-504610176"/>
+        <c:crossAx val="92746496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-504610176"/>
+        <c:axId val="92746496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -673,7 +616,6 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -708,7 +650,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-504596032"/>
+        <c:crossAx val="92744704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -722,7 +664,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -751,7 +692,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1977,7 +1918,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2012,7 +1953,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2189,23 +2130,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2216,36 +2157,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="B2">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="C2">
-        <v>-5</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="B3">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C3">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-10</v>
+        <v>-20</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="B6">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>2</v>

</xml_diff>